<commit_message>
Getting close on ilemt_calibration.docx. Need intro, conclusion, appendix. References are mostly there, and I have reasonable figure layout and page breaks (at the moment).
</commit_message>
<xml_diff>
--- a/calibration/table2_source_fixtures.xlsx
+++ b/calibration/table2_source_fixtures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_papers\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A61DC6-AC84-4155-AECD-682DCAD604F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18191420-55F5-4D05-B445-D10E9EE7FDD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="5760" windowWidth="34560" windowHeight="19140" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="34560" windowHeight="19140" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Table2" sheetId="2" r:id="rId1"/>
@@ -101,7 +101,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +120,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -275,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -334,9 +340,6 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -359,6 +362,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -389,6 +398,9 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="4">
+          <cell r="B4">
+            <v>0.26305582094218294</v>
+          </cell>
           <cell r="F4">
             <v>0.4155529639662352</v>
           </cell>
@@ -810,7 +822,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -823,50 +835,50 @@
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="25" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="25" t="s">
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="28" t="s">
+      <c r="E2" s="29"/>
+      <c r="F2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="28"/>
+      <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="28" t="s">
+      <c r="I2" s="29"/>
+      <c r="J2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29" t="s">
+      <c r="K2" s="28"/>
+      <c r="L2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="29"/>
+      <c r="M2" s="28"/>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
@@ -929,19 +941,19 @@
         <f>'[1]Error stats'!U8</f>
         <v>0.30773206977692641</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="30">
         <f>'[1]Error stats'!F8</f>
         <v>1.8622583486217901</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="30">
         <f>'[1]Error stats'!G8</f>
         <v>5.5141254897433791</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="30">
         <f>'[1]Error stats'!H8</f>
         <v>1.0877705935526274</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="30">
         <f>'[1]Error stats'!I8</f>
         <v>2.8094892492260954</v>
       </c>
@@ -982,19 +994,19 @@
         <f>'[1]Error stats'!U4</f>
         <v>0.50137649258176764</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="31">
         <f>'[1]Error stats'!F4</f>
         <v>0.4155529639662352</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="31">
         <f>'[1]Error stats'!G4</f>
         <v>1.0221359427840411</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="31">
         <f>'[1]Error stats'!H4</f>
         <v>0.27262142803520317</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="31">
         <f>'[1]Error stats'!I4</f>
         <v>0.63741010822327027</v>
       </c>
@@ -1051,19 +1063,19 @@
         <f>'[1]Error stats'!I5</f>
         <v>1.3819778197344657</v>
       </c>
-      <c r="J6" s="23">
+      <c r="J6" s="22">
         <f>'[1]Error stats'!N5</f>
         <v>2.3063463340270505</v>
       </c>
-      <c r="K6" s="24">
+      <c r="K6" s="23">
         <f>'[1]Error stats'!O5</f>
         <v>6.1210123968581813</v>
       </c>
-      <c r="L6" s="24">
+      <c r="L6" s="23">
         <f>'[1]Error stats'!P5</f>
         <v>1.099924631276439</v>
       </c>
-      <c r="M6" s="24">
+      <c r="M6" s="23">
         <f>'[1]Error stats'!Q5</f>
         <v>3.3949064612528712</v>
       </c>

</xml_diff>